<commit_message>
Update vehicle specifications from EV database, Mercedes Benz, Volkswagen
</commit_message>
<xml_diff>
--- a/data/car_specifications.xlsx
+++ b/data/car_specifications.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chrishun\Box Sync\000 Projects IndEcol\90088200 EVD4EUR\X00 EurEVFootprints\Submission files\4 - ERL\code\Zip folder\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chrishun\Box Sync\000 Projects IndEcol\90088200 EVD4EUR\X00 EurEVFootprints\Submission files\code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC04913-9F3A-4BBB-979A-B13791BE220F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084DC9B6-194D-4818-AE8D-AF6A308E2791}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="16320" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>A</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>Production</t>
+  </si>
+  <si>
+    <t>g CO2/km</t>
   </si>
 </sst>
 </file>
@@ -132,7 +135,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -176,11 +179,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,20 +484,17 @@
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D13" sqref="D13:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -659,19 +662,23 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="2">
-        <v>23.736457765667577</v>
-      </c>
-      <c r="E9" s="2">
-        <v>30.98688033233573</v>
-      </c>
-      <c r="F9" s="2">
-        <v>35.047812067271181</v>
-      </c>
-      <c r="G9" s="2">
-        <v>45.788684113548037</v>
+        <v>16</v>
+      </c>
+      <c r="D9" s="4">
+        <f>D11*1000000/180000</f>
+        <v>131.86920980926431</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" ref="E9:G9" si="0">E11*1000000/180000</f>
+        <v>172.14933517964295</v>
+      </c>
+      <c r="F9" s="4">
+        <f t="shared" si="0"/>
+        <v>194.71006704039544</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="0"/>
+        <v>254.38157840860023</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -692,6 +699,26 @@
       </c>
       <c r="G10">
         <v>0.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="2">
+        <v>23.736457765667577</v>
+      </c>
+      <c r="E11" s="2">
+        <v>30.98688033233573</v>
+      </c>
+      <c r="F11" s="2">
+        <v>35.047812067271181</v>
+      </c>
+      <c r="G11" s="2">
+        <v>45.788684113548037</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added single-country real-time footprint functionality.
Fixed sub-annual sampling and added electricity experiment types.
</commit_message>
<xml_diff>
--- a/data/car_specifications.xlsx
+++ b/data/car_specifications.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chrishun\Box Sync\000 Projects IndEcol\90088200 EVD4EUR\X00 EurEVFootprints\Submission files\code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084DC9B6-194D-4818-AE8D-AF6A308E2791}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC09C25-6931-495C-996A-5097E582416B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14760" yWindow="5700" windowWidth="12495" windowHeight="10950" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="alt_energy" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="1" shapeId="0" xr:uid="{50411104-D421-4864-9159-C45E7C9EB28C}">
+    <comment ref="G7" authorId="1" shapeId="0" xr:uid="{50411104-D421-4864-9159-C45E7C9EB28C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -76,8 +78,26 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={7D31461C-9010-4911-9A56-73609FB9C97F}</author>
+  </authors>
+  <commentList>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{7D31461C-9010-4911-9A56-73609FB9C97F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Corresponds to 65 kWhe/kWhc, from Tesla Gigafactory 1 (battery cell production + battery modules and assembly), as per Kurland 2019</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
   <si>
     <t>A</t>
   </si>
@@ -128,6 +148,15 @@
   </si>
   <si>
     <t>g CO2/km</t>
+  </si>
+  <si>
+    <t>cycles</t>
+  </si>
+  <si>
+    <t>km/battery lifetime</t>
+  </si>
+  <si>
+    <t>Max EFC</t>
   </si>
 </sst>
 </file>
@@ -137,7 +166,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +186,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -473,8 +508,16 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="G6" dT="2020-02-11T19:31:54.17" personId="{FDFBB03C-7A38-4EF3-A5B0-64708E03A64A}" id="{50411104-D421-4864-9159-C45E7C9EB28C}">
+  <threadedComment ref="G7" dT="2020-02-11T19:31:54.17" personId="{FDFBB03C-7A38-4EF3-A5B0-64708E03A64A}" id="{50411104-D421-4864-9159-C45E7C9EB28C}">
     <text>WLTP values, average per segment, from EV database</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D2" dT="2021-03-05T12:19:43.23" personId="{FDFBB03C-7A38-4EF3-A5B0-64708E03A64A}" id="{7D31461C-9010-4911-9A56-73609FB9C97F}">
+    <text>Corresponds to 65 kWhe/kWhc, from Tesla Gigafactory 1 (battery cell production + battery modules and assembly), as per Kurland 2019</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -484,16 +527,16 @@
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:J15"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -596,129 +639,356 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1">
-        <v>161.1</v>
-      </c>
-      <c r="E6" s="1">
-        <v>179.2</v>
-      </c>
-      <c r="F6" s="1">
-        <v>172.7</v>
-      </c>
-      <c r="G6" s="1">
-        <v>211</v>
+        <v>17</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1500</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1500</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1500</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1500</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1">
+        <v>161.1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>179.2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>172.7</v>
+      </c>
+      <c r="G7" s="1">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7">
-        <v>0.5</v>
-      </c>
-      <c r="E7">
-        <v>0.7</v>
-      </c>
-      <c r="F7">
-        <v>0.7</v>
-      </c>
-      <c r="G7">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
       <c r="D8">
+        <v>0.5</v>
+      </c>
+      <c r="E8">
+        <v>0.7</v>
+      </c>
+      <c r="F8">
+        <v>0.7</v>
+      </c>
+      <c r="G8">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9">
         <v>3.6</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>5.4</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>8.5</v>
       </c>
-      <c r="G8">
+      <c r="G9">
         <v>10.5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="4">
-        <f>D11*1000000/180000</f>
+      <c r="D10" s="4">
+        <f>D12*1000000/180000</f>
         <v>131.86920980926431</v>
       </c>
-      <c r="E9" s="4">
-        <f t="shared" ref="E9:G9" si="0">E11*1000000/180000</f>
+      <c r="E10" s="4">
+        <f t="shared" ref="E10:G10" si="0">E12*1000000/180000</f>
         <v>172.14933517964295</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F10" s="4">
         <f t="shared" si="0"/>
         <v>194.71006704039544</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G10" s="4">
         <f t="shared" si="0"/>
         <v>254.38157840860023</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10">
-        <v>0.3</v>
-      </c>
-      <c r="E10">
-        <v>0.5</v>
-      </c>
-      <c r="F10">
-        <v>0.6</v>
-      </c>
-      <c r="G10">
-        <v>0.7</v>
-      </c>
-    </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11">
+        <v>0.3</v>
+      </c>
+      <c r="E11">
+        <v>0.5</v>
+      </c>
+      <c r="F11">
+        <v>0.6</v>
+      </c>
+      <c r="G11">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2">
         <v>23.736457765667577</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E12" s="2">
         <v>30.98688033233573</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F12" s="2">
         <v>35.047812067271181</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G12" s="2">
         <v>45.788684113548037</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{040E8226-EE62-48A3-B90B-A28D4879B86C}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A2:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <f>Sheet1!D2</f>
+        <v>26.6</v>
+      </c>
+      <c r="C2">
+        <f>Sheet1!E2</f>
+        <v>42.1</v>
+      </c>
+      <c r="D2">
+        <f>Sheet1!F2</f>
+        <v>59.9</v>
+      </c>
+      <c r="E2">
+        <f>Sheet1!G2</f>
+        <v>89.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <f>Sheet1!D7</f>
+        <v>161.1</v>
+      </c>
+      <c r="C3">
+        <f>Sheet1!E7</f>
+        <v>179.2</v>
+      </c>
+      <c r="D3">
+        <f>Sheet1!F7</f>
+        <v>172.7</v>
+      </c>
+      <c r="E3">
+        <f>Sheet1!G7</f>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>2000</v>
+      </c>
+      <c r="C4">
+        <v>2000</v>
+      </c>
+      <c r="D4">
+        <v>2000</v>
+      </c>
+      <c r="E4">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <f>(AVERAGE(B2,0.8*B2)*1000*B4)/B3</f>
+        <v>297206.70391061454</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:E5" si="0">(C2*1000*C4)/C3</f>
+        <v>469866.07142857148</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>693688.47712796764</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>851184.83412322274</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>1000</v>
+      </c>
+      <c r="C7">
+        <v>1000</v>
+      </c>
+      <c r="D7">
+        <v>1000</v>
+      </c>
+      <c r="E7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <f>(B2*1000*B7)/B3</f>
+        <v>165114.83550589698</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:E8" si="1">(C2*1000*C7)/C3</f>
+        <v>234933.03571428574</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>346844.23856398382</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>425592.41706161137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED4596D-5CE4-4504-93FB-8542EA3EC15C}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
+    <col min="4" max="7" width="10.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <f>65*Sheet1!D2</f>
+        <v>1729</v>
+      </c>
+      <c r="E2">
+        <f>65*Sheet1!E2</f>
+        <v>2736.5</v>
+      </c>
+      <c r="F2">
+        <f>65*Sheet1!F2</f>
+        <v>3893.5</v>
+      </c>
+      <c r="G2">
+        <f>65*Sheet1!G2</f>
+        <v>5837</v>
       </c>
     </row>
   </sheetData>

</xml_diff>